<commit_message>
Changed the excel files so to avoid the loading errors in jupyter files
</commit_message>
<xml_diff>
--- a/Data/MLP/AlN/Sourcecode/Data/RSM-Data.xlsx
+++ b/Data/MLP/AlN/Sourcecode/Data/RSM-Data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karthekeyanperiasamy/Desktop/NeuralNetwork-Code/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karthekeyanperiasamy/Desktop/EC-RSM-ML-Model/Data/MLP/AlN/Sourcecode/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17EDF8A-C2B1-6C4D-A725-8BF8EFE1894F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEA9792-98ED-2E4D-93DD-D0915A30AA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="25040" windowHeight="13880" xr2:uid="{EB1DC66B-A407-9D40-A703-50860373C5D6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data_Final" sheetId="1" r:id="rId1"/>
+    <sheet name="Data-Final" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029" iterate="1"/>
   <extLst>

</xml_diff>